<commit_message>
Modified tests,utility functions and excel file
</commit_message>
<xml_diff>
--- a/src/test/resources/Assignmt 5 test data.xlsx
+++ b/src/test/resources/Assignmt 5 test data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aaroop\IdeaProjects\Rest_Assured_Assignment_5_2024\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C1EEFB8-9FD8-4BFB-8D0D-5790610D5599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0918F0-ABBC-428F-AED6-0C8374A9EC7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="910" yWindow="890" windowWidth="14400" windowHeight="7360" xr2:uid="{5B309D88-D3FA-4E76-B47F-BE5555B01851}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>name</t>
   </si>
@@ -62,7 +62,16 @@
     <t>mini@hhh.yy</t>
   </si>
   <si>
-    <t>mini@hhh.tt</t>
+    <t>male</t>
+  </si>
+  <si>
+    <t>Suresh</t>
+  </si>
+  <si>
+    <t>suresh@hihi.hi</t>
+  </si>
+  <si>
+    <t>active</t>
   </si>
 </sst>
 </file>
@@ -428,7 +437,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -466,22 +475,22 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C2" r:id="rId1" xr:uid="{36757EF3-0EFB-4DAB-AC1A-B6C99C5437A1}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{5BC651B0-6B17-497D-8D1A-DBD4E020A3DF}"/>
+    <hyperlink ref="C3" r:id="rId2" xr:uid="{A9DBC0F0-4A8F-42F1-899D-98C9DA341B3D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>

</xml_diff>